<commit_message>
Updated logs and exception handelling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sweta Kumari\Documents\UiPath\VOIS_EmployeeData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA949EB-FEDE-4C6C-9CFE-0D8444F20631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BCA1EB-84E7-4A3F-B651-00914E5CB418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -186,15 +186,15 @@
     <t>Email_Body</t>
   </si>
   <si>
-    <t>Singh.sweta.n93@gmail.com</t>
-  </si>
-  <si>
     <t>Daily Onboarding Process Report - [Date]</t>
   </si>
   <si>
     <t>⦁ The daily onboarding process has been completed. All Employees Processed: [AllCount]
 ⦁ High Priority Employees Processed: [HighCount]
 ⦁ Normal and Low Employees in Queue: [Count]</t>
+  </si>
+  <si>
+    <t>Email_TO</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
@@ -1842,7 +1842,7 @@
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
         <v>53</v>
@@ -1850,20 +1850,13 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2830,7 +2823,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2841,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
@@ -2929,7 +2921,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>